<commit_message>
Modified ranger Suite data
</commit_message>
<xml_diff>
--- a/data/ExcelData/RangerSuiteData.xlsx
+++ b/data/ExcelData/RangerSuiteData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">LoginAndLogoutUserAdminPage</t>
   </si>
   <si>
-    <t xml:space="preserve">http://dev.ranger9dot5.xpms.ai</t>
+    <t xml:space="preserve">http://dev.ranger.xpms.ai</t>
   </si>
   <si>
     <t xml:space="preserve">admin</t>
@@ -286,18 +286,15 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -390,9 +387,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://dev.ranger9dot5.xpms.ai"/>
-    <hyperlink ref="C3" r:id="rId2" display="http://dev.ranger9dot5.xpms.ai"/>
-    <hyperlink ref="C4" r:id="rId3" display="http://dev.ranger9dot5.xpms.ai"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://dev.ranger.xpms.ai"/>
+    <hyperlink ref="C3" r:id="rId2" display="http://dev.ranger.xpms.ai"/>
+    <hyperlink ref="C4" r:id="rId3" display="http://dev.ranger.xpms.ai"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>